<commit_message>
dynamic header taken done
</commit_message>
<xml_diff>
--- a/BIG-Final.xlsx
+++ b/BIG-Final.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="1016">
   <x:si>
-    <x:t>DivCode</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SubDeptDesc</x:t>
+    <x:t>Div Code</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sub Dept Desc</x:t>
   </x:si>
   <x:si>
     <x:t>Buyer Incharge</x:t>
@@ -28,10 +28,10 @@
     <x:t>No</x:t>
   </x:si>
   <x:si>
-    <x:t>LS Item Code</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item Barcode</x:t>
+    <x:t>Item Code</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barcode</x:t>
   </x:si>
   <x:si>
     <x:t>UOM</x:t>
@@ -61,22 +61,25 @@
     <x:t>Pagination</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> Normal Cost </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Normal RSP </x:t>
+    <x:t>Normal Cost</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Normal RSP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Normal Margin</x:t>
   </x:si>
   <x:si>
     <x:t>Mechanic</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> Promo Cost </x:t>
+    <x:t>Promo Cost</x:t>
   </x:si>
   <x:si>
     <x:t>Nett Promo Cost</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> Promo RSP </x:t>
+    <x:t>Promo RSP</x:t>
   </x:si>
   <x:si>
     <x:t>Promo Margin %</x:t>
@@ -125,9 +128,6 @@
   </x:si>
   <x:si>
     <x:t>Column7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Column8</x:t>
   </x:si>
   <x:si>
     <x:t>D3</x:t>

</xml_diff>